<commit_message>
Add template and completed example
</commit_message>
<xml_diff>
--- a/templates/excel_template_metadata.xlsx
+++ b/templates/excel_template_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinnorgaard/Documents/GitHub/BIDS-converter/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24856A7F-0483-6C4B-A741-EB90F138E873}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09D5AE04-78A9-D04D-B775-9CB3FAD316CC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16700" xr2:uid="{B09AB50C-E81C-BF4B-AB80-4C0F8EC55ACD}"/>
   </bookViews>
@@ -469,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D07A739-95C2-BD46-B2B0-50E40D980EB4}">
   <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>